<commit_message>
add type and option
</commit_message>
<xml_diff>
--- a/기획 데이터 테이블 구성.xlsx
+++ b/기획 데이터 테이블 구성.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nayoonv\game-uruk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75EC32A9-5090-4512-927F-43DA9F9C34B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BA056E-6E4C-41F2-9F60-9B9D0104EAE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11360" yWindow="3490" windowWidth="28800" windowHeight="15500" xr2:uid="{59F6D182-FAEC-4BF3-A690-25A750217E18}"/>
+    <workbookView xWindow="-19632" yWindow="3840" windowWidth="24540" windowHeight="10512" activeTab="1" xr2:uid="{59F6D182-FAEC-4BF3-A690-25A750217E18}"/>
   </bookViews>
   <sheets>
     <sheet name="non_preparations" sheetId="1" r:id="rId1"/>
@@ -452,7 +452,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="207">
   <si>
     <t>NO</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -978,14 +978,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>조수간만 시간(PK)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일자(1~7)(PK)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>지역 id(PK)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1243,6 +1235,49 @@
   </si>
   <si>
     <t>채비 카테고리 id (preparation_id와 preparation_category_id는 복합키이면서 unique키)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>피로도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fatigue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COLUMN_TYPE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COLUMN_OPTION</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR</t>
+  </si>
+  <si>
+    <t>VARCHAR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TINYINT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일자(1~7)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조수간만 시간</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1327,7 +1362,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1361,13 +1396,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1404,16 +1474,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1431,10 +1504,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1734,36 +1803,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3242E66-B909-433E-B55E-F4A11B1BEF69}">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21.83203125" customWidth="1"/>
     <col min="2" max="2" width="22.25" customWidth="1"/>
-    <col min="3" max="3" width="62.5" customWidth="1"/>
+    <col min="3" max="3" width="70.58203125" customWidth="1"/>
+    <col min="4" max="4" width="14.08203125" customWidth="1"/>
+    <col min="5" max="5" width="18.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1773,8 +1850,14 @@
       <c r="C3" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D3" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1784,8 +1867,12 @@
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D4" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1795,8 +1882,12 @@
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D5" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -1806,8 +1897,12 @@
       <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D6" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -1817,27 +1912,37 @@
       <c r="C7" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D7" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A10" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B10" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <v>1</v>
       </c>
@@ -1847,8 +1952,14 @@
       <c r="C11" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D11" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <v>2</v>
       </c>
@@ -1858,8 +1969,12 @@
       <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D12" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <v>3</v>
       </c>
@@ -1869,24 +1984,34 @@
       <c r="C13" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D13" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A16" s="15" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B16" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>1</v>
       </c>
@@ -1896,8 +2021,14 @@
       <c r="C17" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D17" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>2</v>
       </c>
@@ -1907,8 +2038,12 @@
       <c r="C18" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D18" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>3</v>
       </c>
@@ -1918,8 +2053,12 @@
       <c r="C19" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D19" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" s="4">
         <v>4</v>
       </c>
@@ -1929,8 +2068,12 @@
       <c r="C20" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D20" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
         <v>5</v>
       </c>
@@ -1940,8 +2083,12 @@
       <c r="C21" s="6" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D21" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
         <v>6</v>
       </c>
@@ -1951,55 +2098,73 @@
       <c r="C22" s="6" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D22" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" s="4">
         <v>7</v>
       </c>
-      <c r="B23" t="s">
-        <v>163</v>
+      <c r="B23" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D23" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>8</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+        <v>147</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" s="10"/>
-      <c r="B25" s="13"/>
+      <c r="B25" s="16"/>
       <c r="C25" s="11"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A26" s="12" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A26" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C26" s="14"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A27" s="15" t="s">
+      <c r="C26" s="15"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B27" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>1</v>
       </c>
@@ -2007,10 +2172,16 @@
         <v>32</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" s="4">
         <v>2</v>
       </c>
@@ -2018,10 +2189,16 @@
         <v>3</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
         <v>3</v>
       </c>
@@ -2031,8 +2208,12 @@
       <c r="C30" s="6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D30" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
         <v>4</v>
       </c>
@@ -2042,8 +2223,12 @@
       <c r="C31" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D31" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" s="2">
         <v>5</v>
       </c>
@@ -2053,38 +2238,52 @@
       <c r="C32" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D32" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" s="8">
         <v>6</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+        <v>178</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B35" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A36" s="15" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A36" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B36" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B36" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37" s="2">
         <v>1</v>
       </c>
@@ -2094,8 +2293,14 @@
       <c r="C37" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D37" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38" s="2">
         <v>2</v>
       </c>
@@ -2105,8 +2310,12 @@
       <c r="C38" s="2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D38" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>124</v>
       </c>
@@ -2114,18 +2323,24 @@
         <v>125</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A41" s="15" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A41" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B41" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B41" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" s="2">
         <v>1</v>
       </c>
@@ -2133,10 +2348,16 @@
         <v>126</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+        <v>205</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43" s="2">
         <v>2</v>
       </c>
@@ -2144,10 +2365,16 @@
         <v>130</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+        <v>206</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" s="2">
         <v>3</v>
       </c>
@@ -2157,8 +2384,12 @@
       <c r="C44" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D44" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45" s="2">
         <v>4</v>
       </c>
@@ -2166,29 +2397,39 @@
         <v>127</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+        <v>133</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E45" s="2"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B47" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A48" s="15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A48" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B48" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C48" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B48" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" s="2">
         <v>1</v>
       </c>
@@ -2196,10 +2437,16 @@
         <v>32</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50" s="2">
         <v>2</v>
       </c>
@@ -2207,49 +2454,86 @@
         <v>35</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+        <v>187</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B52" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A53" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E53" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A54" s="2">
+        <v>1</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B52" t="s">
+      <c r="D54" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A55" s="2">
+        <v>2</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A53" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B53" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C53" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A54" s="2">
-        <v>1</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A55" s="2">
-        <v>2</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>177</v>
-      </c>
       <c r="C55" s="2" t="s">
-        <v>175</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E55" s="2"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A56" s="2">
+        <v>3</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E56" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2261,10 +2545,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CFF3889-4DE1-4EDC-BE51-A4C2BB00F684}">
-  <dimension ref="A1:C104"/>
+  <dimension ref="A1:E104"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -2272,39 +2556,53 @@
     <col min="1" max="1" width="24.58203125" customWidth="1"/>
     <col min="2" max="2" width="49.58203125" customWidth="1"/>
     <col min="3" max="3" width="75" customWidth="1"/>
+    <col min="4" max="4" width="17.25" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" s="8">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C3" s="8" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="8">
-        <v>1</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D3" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -2312,21 +2610,29 @@
         <v>35</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+        <v>183</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+        <v>157</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -2336,70 +2642,96 @@
       <c r="C6" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D6" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B8" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" s="15" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B9" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D10" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <v>2</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+        <v>186</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A14" s="15" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B14" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <v>1</v>
       </c>
@@ -2407,83 +2739,113 @@
         <v>35</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+        <v>194</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
         <v>2</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D16" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
         <v>3</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+        <v>195</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A20" s="15" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B20" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
         <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22" s="2">
+        <v>2</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22" s="2">
-        <v>2</v>
-      </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D22" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>39</v>
       </c>
@@ -2491,18 +2853,24 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A25" s="15" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B25" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
         <v>1</v>
       </c>
@@ -2512,8 +2880,14 @@
       <c r="C26" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D26" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
         <v>2</v>
       </c>
@@ -2523,8 +2897,12 @@
       <c r="C27" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D27" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" s="2">
         <v>3</v>
       </c>
@@ -2534,8 +2912,12 @@
       <c r="C28" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D28" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
         <v>4</v>
       </c>
@@ -2545,19 +2927,27 @@
       <c r="C29" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D29" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
         <v>5</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D30" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" s="8">
         <v>6</v>
       </c>
@@ -2567,8 +2957,12 @@
       <c r="C31" s="8" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D31" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" s="8">
         <v>7</v>
       </c>
@@ -2578,8 +2972,12 @@
       <c r="C32" s="8" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D32" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" s="8">
         <v>8</v>
       </c>
@@ -2589,13 +2987,17 @@
       <c r="C33" s="8" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D33" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>92</v>
       </c>
@@ -2604,18 +3006,24 @@
       </c>
       <c r="C35" s="9"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A36" s="15" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A36" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B36" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B36" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37" s="8">
         <v>1</v>
       </c>
@@ -2625,8 +3033,14 @@
       <c r="C37" s="8" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D37" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38" s="8">
         <v>2</v>
       </c>
@@ -2636,8 +3050,12 @@
       <c r="C38" s="8" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D38" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>42</v>
       </c>
@@ -2645,18 +3063,24 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A41" s="15" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A41" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B41" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B41" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" s="2">
         <v>1</v>
       </c>
@@ -2666,8 +3090,14 @@
       <c r="C42" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D42" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43" s="2">
         <v>2</v>
       </c>
@@ -2677,8 +3107,12 @@
       <c r="C43" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D43" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" s="2">
         <v>3</v>
       </c>
@@ -2688,8 +3122,12 @@
       <c r="C44" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D44" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E44" s="2"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>52</v>
       </c>
@@ -2697,18 +3135,24 @@
         <v>79</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A47" s="15" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A47" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B47" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48" s="2">
         <v>1</v>
       </c>
@@ -2718,8 +3162,14 @@
       <c r="C48" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D48" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" s="2">
         <v>2</v>
       </c>
@@ -2729,19 +3179,27 @@
       <c r="C49" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D49" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E49" s="2"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50" s="2">
         <v>3</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+        <v>162</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E50" s="2"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" s="2">
         <v>4</v>
       </c>
@@ -2751,8 +3209,12 @@
       <c r="C51" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D51" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E51" s="2"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" s="8">
         <v>5</v>
       </c>
@@ -2762,8 +3224,12 @@
       <c r="C52" s="8" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D52" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E52" s="2"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53" s="8">
         <v>6</v>
       </c>
@@ -2773,8 +3239,12 @@
       <c r="C53" s="8" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D53" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E53" s="2"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>59</v>
       </c>
@@ -2782,18 +3252,24 @@
         <v>80</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A56" s="15" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A56" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B56" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C56" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B56" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D56" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E56" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57" s="2">
         <v>1</v>
       </c>
@@ -2803,8 +3279,14 @@
       <c r="C57" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D57" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58" s="2">
         <v>2</v>
       </c>
@@ -2814,8 +3296,12 @@
       <c r="C58" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D58" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E58" s="2"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59" s="2">
         <v>3</v>
       </c>
@@ -2825,8 +3311,12 @@
       <c r="C59" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D59" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E59" s="2"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A60" s="2">
         <v>4</v>
       </c>
@@ -2836,8 +3326,12 @@
       <c r="C60" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D60" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E60" s="2"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61" s="2">
         <v>5</v>
       </c>
@@ -2845,10 +3339,14 @@
         <v>65</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+        <v>164</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E61" s="2"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
         <v>62</v>
       </c>
@@ -2856,18 +3354,24 @@
         <v>67</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A64" s="15" t="s">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A64" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B64" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C64" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B64" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D64" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E64" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A65" s="2">
         <v>1</v>
       </c>
@@ -2877,8 +3381,14 @@
       <c r="C65" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D65" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A66" s="2">
         <v>2</v>
       </c>
@@ -2888,8 +3398,12 @@
       <c r="C66" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D66" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E66" s="2"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A67" s="2">
         <v>3</v>
       </c>
@@ -2899,8 +3413,12 @@
       <c r="C67" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D67" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E67" s="2"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
         <v>71</v>
       </c>
@@ -2908,18 +3426,24 @@
         <v>81</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A70" s="15" t="s">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A70" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B70" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C70" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B70" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D70" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E70" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A71" s="2">
         <v>1</v>
       </c>
@@ -2929,8 +3453,14 @@
       <c r="C71" s="2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D71" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A72" s="2">
         <v>2</v>
       </c>
@@ -2940,8 +3470,12 @@
       <c r="C72" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D72" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E72" s="2"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A73" s="2">
         <v>3</v>
       </c>
@@ -2951,8 +3485,12 @@
       <c r="C73" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D73" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E73" s="2"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="s">
         <v>75</v>
       </c>
@@ -2960,18 +3498,24 @@
         <v>76</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A76" s="15" t="s">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A76" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B76" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C76" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B76" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C76" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D76" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E76" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A77" s="2">
         <v>1</v>
       </c>
@@ -2981,8 +3525,14 @@
       <c r="C77" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D77" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A78" s="2">
         <v>2</v>
       </c>
@@ -2992,19 +3542,27 @@
       <c r="C78" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D78" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E78" s="2"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A79" s="2">
         <v>3</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D79" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E79" s="2"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A81" s="1" t="s">
         <v>84</v>
       </c>
@@ -3012,18 +3570,24 @@
         <v>89</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A82" s="15" t="s">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A82" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B82" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C82" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B82" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C82" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D82" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E82" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A83" s="2">
         <v>1</v>
       </c>
@@ -3033,8 +3597,14 @@
       <c r="C83" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D83" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A84" s="2">
         <v>2</v>
       </c>
@@ -3042,10 +3612,14 @@
         <v>86</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.45">
+        <v>166</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E84" s="2"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A85" s="8">
         <v>3</v>
       </c>
@@ -3055,8 +3629,12 @@
       <c r="C85" s="8" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D85" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E85" s="2"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A86" s="8">
         <v>4</v>
       </c>
@@ -3066,159 +3644,223 @@
       <c r="C86" s="8" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D86" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E86" s="2"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A88" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B88" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A89" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B89" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C89" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D89" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E89" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A90" s="2">
+        <v>1</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A91" s="2">
+        <v>2</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B88" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A89" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B89" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C89" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A90" s="2">
-        <v>1</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A91" s="2">
-        <v>2</v>
-      </c>
-      <c r="B91" s="2" t="s">
+      <c r="C91" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C91" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D91" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E91" s="2"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A92" s="2">
         <v>3</v>
       </c>
       <c r="B92" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E92" s="2"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A94" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A95" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B95" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C95" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D95" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E95" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A96" s="2">
+        <v>1</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C96" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C92" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A94" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A95" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B95" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C95" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A96" s="2">
-        <v>1</v>
-      </c>
-      <c r="B96" s="2" t="s">
+      <c r="D96" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A97" s="2">
+        <v>2</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="C97" s="2" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A97" s="2">
-        <v>2</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D97" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E97" s="2"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A98" s="2">
         <v>3</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.45">
+        <v>145</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E98" s="2"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A100" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B100" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A101" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B101" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C101" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D101" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E101" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A102" s="2">
+        <v>1</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B100" t="s">
+      <c r="C102" s="2" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A101" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B101" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C101" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A102" s="2">
-        <v>1</v>
-      </c>
-      <c r="B102" s="2" t="s">
+      <c r="D102" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A103" s="2">
+        <v>2</v>
+      </c>
+      <c r="B103" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="C103" s="2" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A103" s="2">
-        <v>2</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D103" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E103" s="2"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A104" s="2">
         <v>3</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>170</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E104" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
delete game data file
</commit_message>
<xml_diff>
--- a/기획 데이터 테이블 구성.xlsx
+++ b/기획 데이터 테이블 구성.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nayoonv\game-uruk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D897B98A-F743-477F-9CDC-CC85D786F974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9A5E48-2C70-4ABA-AF1E-ACC9EDFB3E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{59F6D182-FAEC-4BF3-A690-25A750217E18}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{59F6D182-FAEC-4BF3-A690-25A750217E18}"/>
   </bookViews>
   <sheets>
-    <sheet name="non_preparations" sheetId="1" r:id="rId1"/>
-    <sheet name="preparations" sheetId="2" r:id="rId2"/>
+    <sheet name="game-data" sheetId="3" r:id="rId1"/>
+    <sheet name="product-non-preparations" sheetId="1" r:id="rId2"/>
+    <sheet name="product-preparations" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -452,7 +453,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="277">
   <si>
     <t>NO</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1298,6 +1299,266 @@
   </si>
   <si>
     <t>weight_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>account_user</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인을 위한 사용자 계정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hive_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하이브 id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BIGINT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nation_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>국가 id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>language_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>언어 id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게임 내 유저 id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게임 플레이를 위한 사용자 정보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>레벨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경험치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>골드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pearl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>진주</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_gift_box</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>선물함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유저 id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>received_date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>받은 날짜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DATETIME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_boat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유저의 보로롱24호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boat_level</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보로롱24호 레벨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boat_durability</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보로롱24호 내구도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boat_fuel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보로롱24호 연료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>inventory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인벤토리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>inventory_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인벤토리 id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이템 id (채비일 경우 item_id, 물고기일 경우 fish_id)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get_date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>획득 날짜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>book</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어류 도감</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>catch_date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잡은 날짜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fish_auction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물고기를 사고 판 기록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>누적 골드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sell_date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>판매 날짜 (year함수와 week함수를 사용해서 구분할 예정)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_weather</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유저별 날씨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>날짜, 시간(같은 날짜, 같은 시(hour)이면 )</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>temperature</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>온도 (0~30까지 랜덤 함수로부터 나온 값 저장)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>풍향 id (1~8까지 랜덤 함수로부터 나온 값 저장)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wind_speed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>풍속 (0~20까지 랜덤함수로부터 나온 값 저장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_fish_cost</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유저별 물고기 시세</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>맵 id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가격 (희귀도, 어려운 맵, 크기에 따라 결정됨)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시간 (거래가 이루어지던 시간)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>크기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무게</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1457,7 +1718,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1507,6 +1768,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1822,10 +2086,907 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBF64E5F-28AE-4868-B332-37029AACFFCF}">
+  <dimension ref="A1:E67"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="29.75" customWidth="1"/>
+    <col min="3" max="3" width="55.625" customWidth="1"/>
+    <col min="4" max="4" width="25.25" customWidth="1"/>
+    <col min="5" max="5" width="43.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="B1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="B8" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>2</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>4</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>5</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="B17" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>2</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>3</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="B23" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>2</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>3</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>4</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="B30" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>1</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>2</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>3</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>4</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>5</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="B38" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <v>1</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
+        <v>2</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
+        <v>3</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E42" s="2"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="B44" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
+        <v>1</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
+        <v>2</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E47" s="2"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
+        <v>3</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="B50" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="E51" s="13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
+        <v>1</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="2">
+        <v>2</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="2">
+        <v>3</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E54" s="2"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="2">
+        <v>4</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E55" s="2"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="2">
+        <v>5</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E56" s="2"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="17" t="s">
+        <v>270</v>
+      </c>
+      <c r="B58" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D59" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="E59" s="13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="2">
+        <v>1</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="2">
+        <v>2</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="2">
+        <v>3</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="2">
+        <v>4</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E63" s="2"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="2">
+        <v>5</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="2">
+        <v>6</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E65" s="2"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="2">
+        <v>7</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E66" s="2"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="2">
+        <v>8</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E67" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3242E66-B909-433E-B55E-F4A11B1BEF69}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
@@ -2620,11 +3781,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CFF3889-4DE1-4EDC-BE51-A4C2BB00F684}">
   <dimension ref="A1:E104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>

</xml_diff>